<commit_message>
Probleme a résoudre avec les figure
</commit_message>
<xml_diff>
--- a/Progressions/Informatique_MPSI_PTSI.xlsx
+++ b/Progressions/Informatique_MPSI_PTSI.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Informatique\Progressions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8E162F-902F-4CD9-9D57-671119F793A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DFE9BE-6DE6-4BFE-BA52-38E731D36CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="290" yWindow="490" windowWidth="18910" windowHeight="9320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2022_2023_PTSI" sheetId="1" r:id="rId1"/>
     <sheet name="2022_2023_MPSI" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +24,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
   <si>
     <t>Num</t>
   </si>
@@ -105,13 +108,7 @@
     <t>Structures séquentielles par boucles imbriquées</t>
   </si>
   <si>
-    <t>Fonctions récursives</t>
-  </si>
-  <si>
     <t>Algorithmes gloutons, algorithmes dichotomiques</t>
-  </si>
-  <si>
-    <t>Algorithmes dichotomiques</t>
   </si>
   <si>
     <t>Image cachée</t>
@@ -230,6 +227,92 @@
   <si>
     <t xml:space="preserve">TP_03_Decouverte des listes
 </t>
+  </si>
+  <si>
+    <t>DS 2 + DS 3 (Machine et sur feuille)</t>
+  </si>
+  <si>
+    <t>TP 6 
+Représentation des nombres</t>
+  </si>
+  <si>
+    <t>TP 5
+Traitement d'images</t>
+  </si>
+  <si>
+    <t>Traitement d'images PGM</t>
+  </si>
+  <si>
+    <t>Passage en niveau de gris
+Rotation</t>
+  </si>
+  <si>
+    <t>TP 4
+Boucles imbriquées</t>
+  </si>
+  <si>
+    <t>Percolation d'une grille</t>
+  </si>
+  <si>
+    <t>Exercices sur les listes</t>
+  </si>
+  <si>
+    <t>Structures algorithmiques</t>
+  </si>
+  <si>
+    <t>Rappeles / Initiations
+Exercices sur la création de fonction</t>
+  </si>
+  <si>
+    <t>TP évaluation</t>
+  </si>
+  <si>
+    <t>Activité 7 
+Rendu de monnaie</t>
+  </si>
+  <si>
+    <t>Spécifications, tests, commentaires, annotations</t>
+  </si>
+  <si>
+    <t>TP 7
+Récursivité</t>
+  </si>
+  <si>
+    <t>TP 8
+Algorithmes Gloutons</t>
+  </si>
+  <si>
+    <t>Variant, invariant, complexité</t>
+  </si>
+  <si>
+    <t>TP 9 Algorithmes de tri</t>
+  </si>
+  <si>
+    <t>Activité 6 : 
+Représentation des nombres (Conversions)</t>
+  </si>
+  <si>
+    <t>Problème du sac à dos
+Plus court chemin par un algoritmhe glouton</t>
+  </si>
+  <si>
+    <t>Exercices sur la récursivité</t>
+  </si>
+  <si>
+    <t>Devoir maison (image cachée)
+Activité 8 : Récursivité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité 9 : </t>
+  </si>
+  <si>
+    <t>Tris</t>
+  </si>
+  <si>
+    <t>DS 6</t>
+  </si>
+  <si>
+    <t>DS 7</t>
   </si>
 </sst>
 </file>
@@ -666,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,169 +763,157 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1167,32 +1238,32 @@
   </sheetPr>
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E15" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3:H4"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="F17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="14" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="14" customWidth="1"/>
-    <col min="6" max="8" width="31.81640625" style="16" customWidth="1"/>
-    <col min="9" max="9" width="4.54296875" style="16" customWidth="1"/>
-    <col min="10" max="10" width="31.81640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="5.1796875" style="16" customWidth="1"/>
-    <col min="12" max="13" width="12.453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="3" customWidth="1"/>
+    <col min="6" max="8" width="31.81640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.54296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="31.81640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.1796875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="12.453125" style="2" customWidth="1"/>
     <col min="14" max="15" width="3.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20.81640625" style="3" customWidth="1"/>
     <col min="17" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
@@ -1200,19 +1271,19 @@
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8" t="s">
@@ -1234,21 +1305,21 @@
         <f>B2+6</f>
         <v>44808</v>
       </c>
-      <c r="D2" s="20" t="str">
+      <c r="D2" s="18" t="str">
         <f>CONCATENATE(TEXT(B2,"JJ/MM/AA"),CHAR(10),"au",CHAR(10),TEXT(C2,"JJ/MM/AA"))</f>
         <v>29/08/22
 au
 04/09/22</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
@@ -1263,29 +1334,29 @@
         <f>B3+6</f>
         <v>44815</v>
       </c>
-      <c r="D3" s="20" t="str">
+      <c r="D3" s="18" t="str">
         <f t="shared" ref="D3:D45" si="1">CONCATENATE(TEXT(B3,"JJ/MM/AA"),CHAR(10),"au",CHAR(10),TEXT(C3,"JJ/MM/AA"))</f>
         <v>05/09/22
 au
 11/09/22</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="48">
         <v>1</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
+      <c r="H3" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="13"/>
-      <c r="M3" s="25"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
@@ -1300,21 +1371,21 @@
         <f t="shared" ref="C4:C45" si="3">B4+6</f>
         <v>44822</v>
       </c>
-      <c r="D4" s="20" t="str">
+      <c r="D4" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/09/22
 au
 18/09/22</v>
       </c>
-      <c r="E4" s="46"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="25"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="5" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
@@ -1329,30 +1400,30 @@
         <f t="shared" si="3"/>
         <v>44829</v>
       </c>
-      <c r="D5" s="20" t="str">
+      <c r="D5" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/09/22
 au
 25/09/22</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="48">
         <f>E3+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="26"/>
+      <c r="H5" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
@@ -1367,21 +1438,21 @@
         <f t="shared" si="3"/>
         <v>44836</v>
       </c>
-      <c r="D6" s="20" t="str">
+      <c r="D6" s="18" t="str">
         <f t="shared" si="1"/>
         <v>26/09/22
 au
 02/10/22</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="26"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
@@ -1396,33 +1467,33 @@
         <f t="shared" si="3"/>
         <v>44843</v>
       </c>
-      <c r="D7" s="20" t="str">
+      <c r="D7" s="18" t="str">
         <f t="shared" si="1"/>
         <v>03/10/22
 au
 09/10/22</v>
       </c>
-      <c r="E7" s="45">
+      <c r="E7" s="48">
         <f>E5+1</f>
         <v>3</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="26" t="s">
-        <v>27</v>
+      <c r="G7" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="46"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
@@ -1438,23 +1509,23 @@
         <f t="shared" si="3"/>
         <v>44850</v>
       </c>
-      <c r="D8" s="20" t="str">
+      <c r="D8" s="18" t="str">
         <f t="shared" si="1"/>
         <v>10/10/22
 au
 16/10/22</v>
       </c>
-      <c r="E8" s="46"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="M8" s="26"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
@@ -1468,30 +1539,30 @@
         <f t="shared" si="3"/>
         <v>44857</v>
       </c>
-      <c r="D9" s="20" t="str">
+      <c r="D9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>17/10/22
 au
 23/10/22</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="20">
         <f>E7+1</f>
         <v>4</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="10"/>
     </row>
     <row r="10" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -1503,23 +1574,23 @@
         <f t="shared" si="3"/>
         <v>44864</v>
       </c>
-      <c r="D10" s="20" t="str">
+      <c r="D10" s="18" t="str">
         <f t="shared" si="1"/>
         <v>24/10/22
 au
 30/10/22</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="41"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
@@ -1531,21 +1602,21 @@
         <f t="shared" si="3"/>
         <v>44871</v>
       </c>
-      <c r="D11" s="20" t="str">
+      <c r="D11" s="18" t="str">
         <f t="shared" si="1"/>
         <v>31/10/22
 au
 06/11/22</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43"/>
-      <c r="M11" s="44"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="36"/>
     </row>
     <row r="12" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
@@ -1560,31 +1631,31 @@
         <f t="shared" si="3"/>
         <v>44878</v>
       </c>
-      <c r="D12" s="20" t="str">
+      <c r="D12" s="18" t="str">
         <f t="shared" si="1"/>
         <v>07/11/22
 au
 13/11/22</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <f>E9</f>
         <v>4</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="30" t="s">
+      <c r="G12" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="26" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
@@ -1600,30 +1671,30 @@
         <f t="shared" si="3"/>
         <v>44885</v>
       </c>
-      <c r="D13" s="20" t="str">
+      <c r="D13" s="18" t="str">
         <f t="shared" si="1"/>
         <v>14/11/22
 au
 20/11/22</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="48">
         <f>E12+1</f>
         <v>5</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="26"/>
+      <c r="G13" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="46"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="46"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
@@ -1638,21 +1709,21 @@
         <f t="shared" si="3"/>
         <v>44892</v>
       </c>
-      <c r="D14" s="20" t="str">
+      <c r="D14" s="18" t="str">
         <f t="shared" si="1"/>
         <v>21/11/22
 au
 27/11/22</v>
       </c>
-      <c r="E14" s="46"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="26"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
@@ -1667,28 +1738,28 @@
         <f t="shared" si="3"/>
         <v>44899</v>
       </c>
-      <c r="D15" s="20" t="str">
+      <c r="D15" s="18" t="str">
         <f t="shared" si="1"/>
         <v>28/11/22
 au
 04/12/22</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="48">
         <f>E13+1</f>
         <v>6</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="26"/>
+      <c r="F15" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
@@ -1703,23 +1774,23 @@
         <f t="shared" si="3"/>
         <v>44906</v>
       </c>
-      <c r="D16" s="20" t="str">
+      <c r="D16" s="18" t="str">
         <f t="shared" si="1"/>
         <v>05/12/22
 au
 11/12/22</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="26"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
@@ -1734,30 +1805,30 @@
         <f t="shared" si="3"/>
         <v>44913</v>
       </c>
-      <c r="D17" s="20" t="str">
+      <c r="D17" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/12/22
 au
 18/12/22</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <f>E15+1</f>
         <v>7</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="26" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="26"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="10"/>
     </row>
     <row r="18" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
@@ -1769,23 +1840,23 @@
         <f t="shared" si="3"/>
         <v>44920</v>
       </c>
-      <c r="D18" s="20" t="str">
+      <c r="D18" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/12/22
 au
 25/12/22</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="33"/>
     </row>
     <row r="19" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
@@ -1797,21 +1868,21 @@
         <f t="shared" si="3"/>
         <v>44927</v>
       </c>
-      <c r="D19" s="20" t="str">
+      <c r="D19" s="18" t="str">
         <f t="shared" si="1"/>
         <v>26/12/22
 au
 01/01/23</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="36"/>
     </row>
     <row r="20" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
@@ -1826,20 +1897,20 @@
         <f t="shared" si="3"/>
         <v>44934</v>
       </c>
-      <c r="D20" s="20" t="str">
+      <c r="D20" s="18" t="str">
         <f t="shared" si="1"/>
         <v>02/01/23
 au
 08/01/23</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="20">
         <v>7</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="26" t="s">
         <v>12</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>21</v>
@@ -1847,8 +1918,8 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="26"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="10"/>
     </row>
     <row r="21" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
@@ -1863,30 +1934,30 @@
         <f t="shared" si="3"/>
         <v>44941</v>
       </c>
-      <c r="D21" s="20" t="str">
+      <c r="D21" s="18" t="str">
         <f t="shared" si="1"/>
         <v>09/01/23
 au
 15/01/23</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="48">
         <f>E20+1</f>
         <v>8</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21" s="26"/>
+      <c r="G21" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="10"/>
     </row>
     <row r="22" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
@@ -1901,23 +1972,23 @@
         <f t="shared" si="3"/>
         <v>44948</v>
       </c>
-      <c r="D22" s="20" t="str">
+      <c r="D22" s="18" t="str">
         <f t="shared" si="1"/>
         <v>16/01/23
 au
 22/01/23</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="38" t="s">
-        <v>37</v>
+      <c r="E22" s="49"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="55" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
@@ -1933,29 +2004,29 @@
         <f t="shared" si="3"/>
         <v>44955</v>
       </c>
-      <c r="D23" s="20" t="str">
+      <c r="D23" s="18" t="str">
         <f t="shared" si="1"/>
         <v>23/01/23
 au
 29/01/23</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="48">
         <f>E21+1</f>
         <v>9</v>
       </c>
-      <c r="F23" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="38"/>
+      <c r="F23" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="55"/>
     </row>
     <row r="24" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
@@ -1970,21 +2041,21 @@
         <f t="shared" si="3"/>
         <v>44962</v>
       </c>
-      <c r="D24" s="20" t="str">
+      <c r="D24" s="18" t="str">
         <f t="shared" si="1"/>
         <v>30/01/23
 au
 05/02/23</v>
       </c>
-      <c r="E24" s="46"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="26"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="10"/>
     </row>
     <row r="25" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
@@ -1996,23 +2067,23 @@
         <f t="shared" si="3"/>
         <v>44969</v>
       </c>
-      <c r="D25" s="20" t="str">
+      <c r="D25" s="18" t="str">
         <f t="shared" si="1"/>
         <v>06/02/23
 au
 12/02/23</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="41"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="33"/>
     </row>
     <row r="26" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -2024,21 +2095,21 @@
         <f t="shared" si="3"/>
         <v>44976</v>
       </c>
-      <c r="D26" s="20" t="str">
+      <c r="D26" s="18" t="str">
         <f t="shared" si="1"/>
         <v>13/02/23
 au
 19/02/23</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="36"/>
     </row>
     <row r="27" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
@@ -2053,30 +2124,30 @@
         <f t="shared" si="3"/>
         <v>44983</v>
       </c>
-      <c r="D27" s="20" t="str">
+      <c r="D27" s="18" t="str">
         <f t="shared" si="1"/>
         <v>20/02/23
 au
 26/02/23</v>
       </c>
-      <c r="E27" s="45">
+      <c r="E27" s="48">
         <f>E23+1</f>
         <v>10</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="M27" s="18"/>
+      <c r="G27" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="M27" s="16"/>
     </row>
     <row r="28" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
@@ -2091,21 +2162,21 @@
         <f t="shared" si="3"/>
         <v>44990</v>
       </c>
-      <c r="D28" s="20" t="str">
+      <c r="D28" s="18" t="str">
         <f t="shared" si="1"/>
         <v>27/02/23
 au
 05/03/23</v>
       </c>
-      <c r="E28" s="46"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="18"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
@@ -2120,28 +2191,28 @@
         <f t="shared" si="3"/>
         <v>44997</v>
       </c>
-      <c r="D29" s="20" t="str">
+      <c r="D29" s="18" t="str">
         <f t="shared" si="1"/>
         <v>06/03/23
 au
 12/03/23</v>
       </c>
-      <c r="E29" s="45">
+      <c r="E29" s="48">
         <f>E27+1</f>
         <v>11</v>
       </c>
-      <c r="F29" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="26"/>
+      <c r="F29" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
@@ -2156,21 +2227,21 @@
         <f t="shared" si="3"/>
         <v>45004</v>
       </c>
-      <c r="D30" s="20" t="str">
+      <c r="D30" s="18" t="str">
         <f t="shared" si="1"/>
         <v>13/03/23
 au
 19/03/23</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="30"/>
-      <c r="M30" s="26"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="47"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="10"/>
     </row>
     <row r="31" spans="1:16" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
@@ -2185,27 +2256,27 @@
         <f t="shared" si="3"/>
         <v>45011</v>
       </c>
-      <c r="D31" s="20" t="str">
+      <c r="D31" s="18" t="str">
         <f t="shared" si="1"/>
         <v>20/03/23
 au
 26/03/23</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="48">
         <f>E29+1</f>
         <v>12</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="35"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="46"/>
       <c r="L31" s="13"/>
-      <c r="M31" s="25" t="s">
-        <v>29</v>
+      <c r="M31" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="P31" s="4"/>
     </row>
@@ -2222,21 +2293,21 @@
         <f t="shared" si="3"/>
         <v>45018</v>
       </c>
-      <c r="D32" s="20" t="str">
+      <c r="D32" s="18" t="str">
         <f t="shared" si="1"/>
         <v>27/03/23
 au
 02/04/23</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="36"/>
+      <c r="E32" s="49"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="47"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="25"/>
+      <c r="M32" s="23"/>
     </row>
     <row r="33" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
@@ -2250,27 +2321,27 @@
         <f t="shared" si="3"/>
         <v>45025</v>
       </c>
-      <c r="D33" s="20" t="str">
+      <c r="D33" s="18" t="str">
         <f t="shared" si="1"/>
         <v>03/04/23
 au
 09/04/23</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="20">
         <v>13</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="30"/>
+      <c r="H33" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="26"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="25"/>
+      <c r="M33" s="23"/>
     </row>
     <row r="34" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
@@ -2282,23 +2353,23 @@
         <f t="shared" si="3"/>
         <v>45032</v>
       </c>
-      <c r="D34" s="20" t="str">
+      <c r="D34" s="18" t="str">
         <f t="shared" si="1"/>
         <v>10/04/23
 au
 16/04/23</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="56"/>
-      <c r="M34" s="57"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="42"/>
     </row>
     <row r="35" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
@@ -2310,21 +2381,21 @@
         <f t="shared" si="3"/>
         <v>45039</v>
       </c>
-      <c r="D35" s="20" t="str">
+      <c r="D35" s="18" t="str">
         <f t="shared" si="1"/>
         <v>17/04/23
 au
 23/04/23</v>
       </c>
-      <c r="E35" s="48"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="59"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="45"/>
     </row>
     <row r="36" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
@@ -2336,28 +2407,28 @@
         <f t="shared" si="3"/>
         <v>45046</v>
       </c>
-      <c r="D36" s="20" t="str">
+      <c r="D36" s="18" t="str">
         <f t="shared" si="1"/>
         <v>24/04/23
 au
 30/04/23</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="20">
         <v>13</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="I36" s="30"/>
+      <c r="H36" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36" s="26"/>
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
-      <c r="L36" s="28"/>
-      <c r="M36" s="25" t="s">
-        <v>30</v>
+      <c r="L36" s="25"/>
+      <c r="M36" s="23" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
@@ -2370,28 +2441,28 @@
         <f t="shared" si="3"/>
         <v>45053</v>
       </c>
-      <c r="D37" s="20" t="str">
+      <c r="D37" s="18" t="str">
         <f t="shared" si="1"/>
         <v>01/05/23
 au
 07/05/23</v>
       </c>
-      <c r="E37" s="45">
+      <c r="E37" s="48">
         <f>E36+1</f>
         <v>14</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="35"/>
-      <c r="H37" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="35"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="26"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="46"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="26"/>
+      <c r="M37" s="10"/>
     </row>
     <row r="38" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
@@ -2403,21 +2474,21 @@
         <f t="shared" si="3"/>
         <v>45060</v>
       </c>
-      <c r="D38" s="20" t="str">
+      <c r="D38" s="18" t="str">
         <f t="shared" si="1"/>
         <v>08/05/23
 au
 14/05/23</v>
       </c>
-      <c r="E38" s="46"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="26"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="10"/>
     </row>
     <row r="39" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
@@ -2429,30 +2500,30 @@
         <f t="shared" si="3"/>
         <v>45067</v>
       </c>
-      <c r="D39" s="20" t="str">
+      <c r="D39" s="18" t="str">
         <f t="shared" si="1"/>
         <v>15/05/23
 au
 21/05/23</v>
       </c>
-      <c r="E39" s="45">
+      <c r="E39" s="48">
         <f>E37+1</f>
         <v>15</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="35"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="L39" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="M39" s="26"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="L39" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="M39" s="10"/>
     </row>
     <row r="40" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
@@ -2464,21 +2535,21 @@
         <f t="shared" si="3"/>
         <v>45074</v>
       </c>
-      <c r="D40" s="20" t="str">
+      <c r="D40" s="18" t="str">
         <f t="shared" si="1"/>
         <v>22/05/23
 au
 28/05/23</v>
       </c>
-      <c r="E40" s="46"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="26"/>
+      <c r="E40" s="49"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="10"/>
     </row>
     <row r="41" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
@@ -2490,28 +2561,28 @@
         <f t="shared" si="3"/>
         <v>45081</v>
       </c>
-      <c r="D41" s="20" t="str">
+      <c r="D41" s="18" t="str">
         <f t="shared" si="1"/>
         <v>29/05/23
 au
 04/06/23</v>
       </c>
-      <c r="E41" s="45">
+      <c r="E41" s="48">
         <f>E39+1</f>
         <v>16</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="35"/>
-      <c r="H41" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="35"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="35"/>
-      <c r="L41" s="30"/>
-      <c r="M41" s="26"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="46"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="10"/>
     </row>
     <row r="42" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
@@ -2523,22 +2594,22 @@
         <f t="shared" si="3"/>
         <v>45088</v>
       </c>
-      <c r="D42" s="20" t="str">
+      <c r="D42" s="18" t="str">
         <f t="shared" si="1"/>
         <v>05/06/23
 au
 11/06/23</v>
       </c>
-      <c r="E42" s="46"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="30"/>
-      <c r="M42" s="26" t="s">
-        <v>35</v>
+      <c r="E42" s="49"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="31.5" x14ac:dyDescent="0.35">
@@ -2551,24 +2622,24 @@
         <f t="shared" si="3"/>
         <v>45095</v>
       </c>
-      <c r="D43" s="20" t="str">
+      <c r="D43" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/06/23
 au
 18/06/23</v>
       </c>
-      <c r="E43" s="47">
+      <c r="E43" s="40">
         <f>E41+1</f>
         <v>17</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="37"/>
-      <c r="L43" s="27" t="s">
-        <v>45</v>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="M43" s="10"/>
     </row>
@@ -2582,20 +2653,20 @@
         <f t="shared" si="3"/>
         <v>45102</v>
       </c>
-      <c r="D44" s="20" t="str">
+      <c r="D44" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/06/23
 au
 25/06/23</v>
       </c>
-      <c r="E44" s="48"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="33"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="29"/>
       <c r="M44" s="10"/>
     </row>
     <row r="45" spans="1:13" ht="32" thickBot="1" x14ac:dyDescent="0.4">
@@ -2608,177 +2679,257 @@
         <f t="shared" si="3"/>
         <v>45109</v>
       </c>
-      <c r="D45" s="21" t="str">
+      <c r="D45" s="19" t="str">
         <f t="shared" si="1"/>
         <v>26/06/23
 au
 02/07/23</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="21">
         <f>E43+1</f>
         <v>18</v>
       </c>
-      <c r="F45" s="51"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
-      <c r="L45" s="24"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+      <c r="L45" s="22"/>
       <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B46" s="15"/>
+      <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B47" s="15"/>
+      <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B48" s="15"/>
+      <c r="B48" s="14"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="15"/>
+      <c r="B49" s="14"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="15"/>
+      <c r="B50" s="14"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="15"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="15"/>
+      <c r="B52" s="14"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="15"/>
+      <c r="B53" s="14"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="15"/>
+      <c r="B54" s="14"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="15"/>
+      <c r="B55" s="14"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="15"/>
+      <c r="B56" s="14"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="15"/>
+      <c r="B57" s="14"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="15"/>
+      <c r="B58" s="14"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="15"/>
+      <c r="B59" s="14"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="15"/>
+      <c r="B60" s="14"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="15"/>
+      <c r="B61" s="14"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="15"/>
+      <c r="B62" s="14"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
+      <c r="B63" s="14"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="15"/>
+      <c r="B64" s="14"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="15"/>
+      <c r="B65" s="14"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="15"/>
+      <c r="B66" s="14"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="15"/>
+      <c r="B67" s="14"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="15"/>
+      <c r="B68" s="14"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="15"/>
+      <c r="B69" s="14"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" s="15"/>
+      <c r="B70" s="14"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="15"/>
+      <c r="B71" s="14"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" s="15"/>
+      <c r="B72" s="14"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="15"/>
+      <c r="B73" s="14"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="15"/>
+      <c r="B74" s="14"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="15"/>
+      <c r="B75" s="14"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="15"/>
+      <c r="B76" s="14"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="15"/>
+      <c r="B77" s="14"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="15"/>
+      <c r="B78" s="14"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="15"/>
+      <c r="B79" s="14"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" s="15"/>
+      <c r="B80" s="14"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="15"/>
+      <c r="B81" s="14"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="15"/>
+      <c r="B82" s="14"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="15"/>
+      <c r="B83" s="14"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="15"/>
+      <c r="B84" s="14"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" s="15"/>
+      <c r="B85" s="14"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="15"/>
+      <c r="B86" s="14"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" s="15"/>
+      <c r="B87" s="14"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="15"/>
+      <c r="B88" s="14"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="15"/>
+      <c r="B89" s="14"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="15"/>
+      <c r="B90" s="14"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" s="15"/>
+      <c r="B91" s="14"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="15"/>
+      <c r="B92" s="14"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="15"/>
+      <c r="B93" s="14"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" s="15"/>
+      <c r="B94" s="14"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="15"/>
+      <c r="B95" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="96">
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K31:K32"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="K23:K24"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="E18:M19"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
     <mergeCell ref="E10:M11"/>
     <mergeCell ref="E2:M2"/>
     <mergeCell ref="E25:M26"/>
@@ -2795,86 +2946,6 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="E18:M19"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="I31:I32"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="I23:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -2888,30 +2959,30 @@
   </sheetPr>
   <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:L2"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="13" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="14" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="14" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="14" customWidth="1"/>
-    <col min="6" max="9" width="31.81640625" style="16" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="16" customWidth="1"/>
-    <col min="11" max="12" width="12.453125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="3" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="3" customWidth="1"/>
+    <col min="6" max="9" width="31.81640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="2" customWidth="1"/>
+    <col min="11" max="12" width="12.453125" style="2" customWidth="1"/>
     <col min="13" max="14" width="3.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.81640625" style="3" customWidth="1"/>
     <col min="16" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
@@ -2919,18 +2990,18 @@
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J1" s="8"/>
       <c r="K1" s="8" t="s">
@@ -2952,20 +3023,20 @@
         <f>B2+6</f>
         <v>44808</v>
       </c>
-      <c r="D2" s="20" t="str">
+      <c r="D2" s="18" t="str">
         <f>CONCATENATE(TEXT(B2,"JJ/MM/AA"),CHAR(10),"au",CHAR(10),TEXT(C2,"JJ/MM/AA"))</f>
         <v>29/08/22
 au
 04/09/22</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="55"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39"/>
     </row>
     <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
@@ -2980,26 +3051,28 @@
         <f>B3+6</f>
         <v>44815</v>
       </c>
-      <c r="D3" s="20" t="str">
+      <c r="D3" s="18" t="str">
         <f t="shared" ref="D3:D45" si="1">CONCATENATE(TEXT(B3,"JJ/MM/AA"),CHAR(10),"au",CHAR(10),TEXT(C3,"JJ/MM/AA"))</f>
         <v>05/09/22
 au
 11/09/22</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="40">
         <v>1</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="30"/>
+      <c r="H3" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="52"/>
+      <c r="J3" s="26"/>
       <c r="K3" s="13"/>
-      <c r="L3" s="25"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
@@ -3014,20 +3087,20 @@
         <f t="shared" ref="C4:C45" si="3">B4+6</f>
         <v>44822</v>
       </c>
-      <c r="D4" s="20" t="str">
+      <c r="D4" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/09/22
 au
 18/09/22</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="30"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="26"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="25"/>
+      <c r="L4" s="23"/>
     </row>
     <row r="5" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
@@ -3042,27 +3115,29 @@
         <f t="shared" si="3"/>
         <v>44829</v>
       </c>
-      <c r="D5" s="20" t="str">
+      <c r="D5" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/09/22
 au
 25/09/22</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="40">
         <f>E3+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="G5" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="26"/>
+      <c r="H5" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="52"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="10"/>
     </row>
     <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
@@ -3077,20 +3152,20 @@
         <f t="shared" si="3"/>
         <v>44836</v>
       </c>
-      <c r="D6" s="20" t="str">
+      <c r="D6" s="18" t="str">
         <f t="shared" si="1"/>
         <v>26/09/22
 au
 02/10/22</v>
       </c>
-      <c r="E6" s="48"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="26"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="10"/>
     </row>
     <row r="7" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
@@ -3105,28 +3180,30 @@
         <f t="shared" si="3"/>
         <v>44843</v>
       </c>
-      <c r="D7" s="20" t="str">
+      <c r="D7" s="18" t="str">
         <f t="shared" si="1"/>
         <v>03/10/22
 au
 09/10/22</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="40">
         <f>E5+1</f>
         <v>3</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="37" t="s">
+      <c r="G7" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="26" t="s">
-        <v>27</v>
+      <c r="H7" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="52"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
@@ -3142,22 +3219,22 @@
         <f t="shared" si="3"/>
         <v>44850</v>
       </c>
-      <c r="D8" s="20" t="str">
+      <c r="D8" s="18" t="str">
         <f t="shared" si="1"/>
         <v>10/10/22
 au
 16/10/22</v>
       </c>
-      <c r="E8" s="48"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="26"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
@@ -3171,29 +3248,29 @@
         <f t="shared" si="3"/>
         <v>44857</v>
       </c>
-      <c r="D9" s="20" t="str">
+      <c r="D9" s="18" t="str">
         <f t="shared" si="1"/>
         <v>17/10/22
 au
 23/10/22</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="20">
         <f>E7+1</f>
         <v>4</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="26"/>
+      <c r="G9" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
@@ -3205,22 +3282,22 @@
         <f t="shared" si="3"/>
         <v>44864</v>
       </c>
-      <c r="D10" s="20" t="str">
+      <c r="D10" s="18" t="str">
         <f t="shared" si="1"/>
         <v>24/10/22
 au
 30/10/22</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="41"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
     </row>
     <row r="11" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
@@ -3232,22 +3309,22 @@
         <f t="shared" si="3"/>
         <v>44871</v>
       </c>
-      <c r="D11" s="20" t="str">
+      <c r="D11" s="18" t="str">
         <f t="shared" si="1"/>
         <v>31/10/22
 au
 06/11/22</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="44"/>
-    </row>
-    <row r="12" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:12" ht="39" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <f>A9+1</f>
         <v>8</v>
@@ -3260,30 +3337,32 @@
         <f t="shared" si="3"/>
         <v>44878</v>
       </c>
-      <c r="D12" s="20" t="str">
+      <c r="D12" s="18" t="str">
         <f t="shared" si="1"/>
         <v>07/11/22
 au
 13/11/22</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="20">
         <f>E9</f>
         <v>4</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="26" t="s">
-        <v>28</v>
+      <c r="G12" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="10" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
@@ -3299,29 +3378,29 @@
         <f t="shared" si="3"/>
         <v>44885</v>
       </c>
-      <c r="D13" s="20" t="str">
+      <c r="D13" s="18" t="str">
         <f t="shared" si="1"/>
         <v>14/11/22
 au
 20/11/22</v>
       </c>
-      <c r="E13" s="47">
+      <c r="E13" s="48">
         <f>E12+1</f>
         <v>5</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="37"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="26"/>
+      <c r="G13" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="47"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="10"/>
     </row>
     <row r="14" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
@@ -3336,20 +3415,26 @@
         <f t="shared" si="3"/>
         <v>44892</v>
       </c>
-      <c r="D14" s="20" t="str">
+      <c r="D14" s="18" t="str">
         <f t="shared" si="1"/>
         <v>21/11/22
 au
 27/11/22</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="26"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="46" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="10"/>
     </row>
     <row r="15" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
@@ -3364,27 +3449,25 @@
         <f t="shared" si="3"/>
         <v>44899</v>
       </c>
-      <c r="D15" s="20" t="str">
+      <c r="D15" s="18" t="str">
         <f t="shared" si="1"/>
         <v>28/11/22
 au
 04/12/22</v>
       </c>
-      <c r="E15" s="47">
+      <c r="E15" s="40">
         <f>E13+1</f>
         <v>6</v>
       </c>
-      <c r="F15" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="26"/>
+      <c r="F15" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
@@ -3399,22 +3482,28 @@
         <f t="shared" si="3"/>
         <v>44906</v>
       </c>
-      <c r="D16" s="20" t="str">
+      <c r="D16" s="18" t="str">
         <f t="shared" si="1"/>
         <v>05/12/22
 au
 11/12/22</v>
       </c>
-      <c r="E16" s="48"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="26"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
@@ -3429,27 +3518,25 @@
         <f t="shared" si="3"/>
         <v>44913</v>
       </c>
-      <c r="D17" s="20" t="str">
+      <c r="D17" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/12/22
 au
 18/12/22</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="20">
         <f>E15+1</f>
         <v>7</v>
       </c>
-      <c r="F17" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
+      <c r="F17" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="26"/>
+      <c r="K17" s="26"/>
+      <c r="L17" s="10"/>
     </row>
     <row r="18" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
@@ -3461,22 +3548,22 @@
         <f t="shared" si="3"/>
         <v>44920</v>
       </c>
-      <c r="D18" s="20" t="str">
+      <c r="D18" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/12/22
 au
 25/12/22</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="33"/>
     </row>
     <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
@@ -3488,20 +3575,20 @@
         <f t="shared" si="3"/>
         <v>44927</v>
       </c>
-      <c r="D19" s="20" t="str">
+      <c r="D19" s="18" t="str">
         <f t="shared" si="1"/>
         <v>26/12/22
 au
 01/01/23</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36"/>
     </row>
     <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
@@ -3516,26 +3603,30 @@
         <f t="shared" si="3"/>
         <v>44934</v>
       </c>
-      <c r="D20" s="20" t="str">
+      <c r="D20" s="18" t="str">
         <f t="shared" si="1"/>
         <v>02/01/23
 au
 08/01/23</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="20">
         <v>7</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
+      <c r="F20" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="I20" s="46" t="s">
+        <v>81</v>
+      </c>
       <c r="J20" s="13"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="26"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="10"/>
     </row>
     <row r="21" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
@@ -3550,29 +3641,27 @@
         <f t="shared" si="3"/>
         <v>44941</v>
       </c>
-      <c r="D21" s="20" t="str">
+      <c r="D21" s="18" t="str">
         <f t="shared" si="1"/>
         <v>09/01/23
 au
 15/01/23</v>
       </c>
-      <c r="E21" s="47">
+      <c r="E21" s="40">
         <f>E20+1</f>
         <v>8</v>
       </c>
-      <c r="F21" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21" s="26"/>
+      <c r="F21" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
@@ -3587,22 +3676,28 @@
         <f t="shared" si="3"/>
         <v>44948</v>
       </c>
-      <c r="D22" s="20" t="str">
+      <c r="D22" s="18" t="str">
         <f t="shared" si="1"/>
         <v>16/01/23
 au
 22/01/23</v>
       </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="38" t="s">
-        <v>37</v>
+      <c r="E22" s="43"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="55" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
@@ -3618,26 +3713,26 @@
         <f t="shared" si="3"/>
         <v>44955</v>
       </c>
-      <c r="D23" s="20" t="str">
+      <c r="D23" s="18" t="str">
         <f t="shared" si="1"/>
         <v>23/01/23
 au
 29/01/23</v>
       </c>
-      <c r="E23" s="47">
+      <c r="E23" s="40">
         <f>E21+1</f>
         <v>9</v>
       </c>
-      <c r="F23" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="38"/>
+      <c r="F23" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="55"/>
     </row>
     <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
@@ -3652,20 +3747,26 @@
         <f t="shared" si="3"/>
         <v>44962</v>
       </c>
-      <c r="D24" s="20" t="str">
+      <c r="D24" s="18" t="str">
         <f t="shared" si="1"/>
         <v>30/01/23
 au
 05/02/23</v>
       </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="26"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
@@ -3677,22 +3778,22 @@
         <f t="shared" si="3"/>
         <v>44969</v>
       </c>
-      <c r="D25" s="20" t="str">
+      <c r="D25" s="18" t="str">
         <f t="shared" si="1"/>
         <v>06/02/23
 au
 12/02/23</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="41"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="33"/>
     </row>
     <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -3704,20 +3805,20 @@
         <f t="shared" si="3"/>
         <v>44976</v>
       </c>
-      <c r="D26" s="20" t="str">
+      <c r="D26" s="18" t="str">
         <f t="shared" si="1"/>
         <v>13/02/23
 au
 19/02/23</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="44"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
@@ -3732,29 +3833,29 @@
         <f t="shared" si="3"/>
         <v>44983</v>
       </c>
-      <c r="D27" s="20" t="str">
+      <c r="D27" s="18" t="str">
         <f t="shared" si="1"/>
         <v>20/02/23
 au
 26/02/23</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="40">
         <f>E23+1</f>
         <v>10</v>
       </c>
-      <c r="F27" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="H27" s="37"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L27" s="18"/>
+      <c r="F27" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="52"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L27" s="16"/>
     </row>
     <row r="28" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
@@ -3769,20 +3870,20 @@
         <f t="shared" si="3"/>
         <v>44990</v>
       </c>
-      <c r="D28" s="20" t="str">
+      <c r="D28" s="18" t="str">
         <f t="shared" si="1"/>
         <v>27/02/23
 au
 05/03/23</v>
       </c>
-      <c r="E28" s="48"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="18"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="16"/>
     </row>
     <row r="29" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
@@ -3797,27 +3898,27 @@
         <f t="shared" si="3"/>
         <v>44997</v>
       </c>
-      <c r="D29" s="20" t="str">
+      <c r="D29" s="18" t="str">
         <f t="shared" si="1"/>
         <v>06/03/23
 au
 12/03/23</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="40">
         <f>E27+1</f>
         <v>11</v>
       </c>
-      <c r="F29" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="G29" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="37"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="26"/>
+      <c r="F29" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="52"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
@@ -3832,20 +3933,20 @@
         <f t="shared" si="3"/>
         <v>45004</v>
       </c>
-      <c r="D30" s="20" t="str">
+      <c r="D30" s="18" t="str">
         <f t="shared" si="1"/>
         <v>13/03/23
 au
 19/03/23</v>
       </c>
-      <c r="E30" s="48"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="30"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="26"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="10"/>
     </row>
     <row r="31" spans="1:15" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
@@ -3860,26 +3961,26 @@
         <f t="shared" si="3"/>
         <v>45011</v>
       </c>
-      <c r="D31" s="20" t="str">
+      <c r="D31" s="18" t="str">
         <f t="shared" si="1"/>
         <v>20/03/23
 au
 26/03/23</v>
       </c>
-      <c r="E31" s="47">
+      <c r="E31" s="40">
         <f>E29+1</f>
         <v>12</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
       <c r="K31" s="13"/>
-      <c r="L31" s="25" t="s">
-        <v>29</v>
+      <c r="L31" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="O31" s="4"/>
     </row>
@@ -3896,20 +3997,20 @@
         <f t="shared" si="3"/>
         <v>45018</v>
       </c>
-      <c r="D32" s="20" t="str">
+      <c r="D32" s="18" t="str">
         <f t="shared" si="1"/>
         <v>27/03/23
 au
 02/04/23</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
       <c r="K32" s="13"/>
-      <c r="L32" s="25"/>
+      <c r="L32" s="23"/>
     </row>
     <row r="33" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
@@ -3923,26 +4024,26 @@
         <f t="shared" si="3"/>
         <v>45025</v>
       </c>
-      <c r="D33" s="20" t="str">
+      <c r="D33" s="18" t="str">
         <f t="shared" si="1"/>
         <v>03/04/23
 au
 09/04/23</v>
       </c>
-      <c r="E33" s="22">
+      <c r="E33" s="20">
         <v>13</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="13"/>
-      <c r="H33" s="30" t="s">
-        <v>40</v>
+      <c r="H33" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
-      <c r="L33" s="25"/>
+      <c r="L33" s="23"/>
     </row>
     <row r="34" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
@@ -3954,22 +4055,22 @@
         <f t="shared" si="3"/>
         <v>45032</v>
       </c>
-      <c r="D34" s="20" t="str">
+      <c r="D34" s="18" t="str">
         <f t="shared" si="1"/>
         <v>10/04/23
 au
 16/04/23</v>
       </c>
-      <c r="E34" s="47" t="s">
+      <c r="E34" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="56"/>
-      <c r="G34" s="56"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="56"/>
-      <c r="J34" s="56"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="57"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="42"/>
     </row>
     <row r="35" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
@@ -3981,20 +4082,20 @@
         <f t="shared" si="3"/>
         <v>45039</v>
       </c>
-      <c r="D35" s="20" t="str">
+      <c r="D35" s="18" t="str">
         <f t="shared" si="1"/>
         <v>17/04/23
 au
 23/04/23</v>
       </c>
-      <c r="E35" s="48"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="59"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="45"/>
     </row>
     <row r="36" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
@@ -4006,27 +4107,27 @@
         <f t="shared" si="3"/>
         <v>45046</v>
       </c>
-      <c r="D36" s="20" t="str">
+      <c r="D36" s="18" t="str">
         <f t="shared" si="1"/>
         <v>24/04/23
 au
 30/04/23</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="20">
         <v>13</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G36" s="13"/>
-      <c r="H36" s="30" t="s">
-        <v>40</v>
+      <c r="H36" s="26" t="s">
+        <v>38</v>
       </c>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
-      <c r="K36" s="28"/>
-      <c r="L36" s="25" t="s">
-        <v>30</v>
+      <c r="K36" s="25"/>
+      <c r="L36" s="23" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
@@ -4039,27 +4140,27 @@
         <f t="shared" si="3"/>
         <v>45053</v>
       </c>
-      <c r="D37" s="20" t="str">
+      <c r="D37" s="18" t="str">
         <f t="shared" si="1"/>
         <v>01/05/23
 au
 07/05/23</v>
       </c>
-      <c r="E37" s="47">
+      <c r="E37" s="40">
         <f>E36+1</f>
         <v>14</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37" t="s">
-        <v>42</v>
-      </c>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="26"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="10"/>
     </row>
     <row r="38" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
@@ -4071,20 +4172,20 @@
         <f t="shared" si="3"/>
         <v>45060</v>
       </c>
-      <c r="D38" s="20" t="str">
+      <c r="D38" s="18" t="str">
         <f t="shared" si="1"/>
         <v>08/05/23
 au
 14/05/23</v>
       </c>
-      <c r="E38" s="48"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="26"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+      <c r="L38" s="10"/>
     </row>
     <row r="39" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
@@ -4096,29 +4197,29 @@
         <f t="shared" si="3"/>
         <v>45067</v>
       </c>
-      <c r="D39" s="20" t="str">
+      <c r="D39" s="18" t="str">
         <f t="shared" si="1"/>
         <v>15/05/23
 au
 21/05/23</v>
       </c>
-      <c r="E39" s="47">
+      <c r="E39" s="40">
         <f>E37+1</f>
         <v>15</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F39" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="37"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="K39" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="L39" s="26"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L39" s="10"/>
     </row>
     <row r="40" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
@@ -4130,20 +4231,20 @@
         <f t="shared" si="3"/>
         <v>45074</v>
       </c>
-      <c r="D40" s="20" t="str">
+      <c r="D40" s="18" t="str">
         <f t="shared" si="1"/>
         <v>22/05/23
 au
 28/05/23</v>
       </c>
-      <c r="E40" s="48"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="26"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="10"/>
     </row>
     <row r="41" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
@@ -4155,27 +4256,27 @@
         <f t="shared" si="3"/>
         <v>45081</v>
       </c>
-      <c r="D41" s="20" t="str">
+      <c r="D41" s="18" t="str">
         <f t="shared" si="1"/>
         <v>29/05/23
 au
 04/06/23</v>
       </c>
-      <c r="E41" s="47">
+      <c r="E41" s="40">
         <f>E39+1</f>
         <v>16</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="I41" s="30"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="30"/>
-      <c r="L41" s="26"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="10"/>
     </row>
     <row r="42" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
@@ -4187,21 +4288,21 @@
         <f t="shared" si="3"/>
         <v>45088</v>
       </c>
-      <c r="D42" s="20" t="str">
+      <c r="D42" s="18" t="str">
         <f t="shared" si="1"/>
         <v>05/06/23
 au
 11/06/23</v>
       </c>
-      <c r="E42" s="48"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
-      <c r="K42" s="30"/>
-      <c r="L42" s="26" t="s">
-        <v>35</v>
+      <c r="E42" s="43"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="10" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
@@ -4214,25 +4315,25 @@
         <f t="shared" si="3"/>
         <v>45095</v>
       </c>
-      <c r="D43" s="20" t="str">
+      <c r="D43" s="18" t="str">
         <f t="shared" si="1"/>
         <v>12/06/23
 au
 18/06/23</v>
       </c>
-      <c r="E43" s="47">
+      <c r="E43" s="40">
         <f>E41+1</f>
         <v>17</v>
       </c>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
-      <c r="K43" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="L43" s="26"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="L43" s="10"/>
     </row>
     <row r="44" spans="1:12" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
@@ -4244,20 +4345,20 @@
         <f t="shared" si="3"/>
         <v>45102</v>
       </c>
-      <c r="D44" s="20" t="str">
+      <c r="D44" s="18" t="str">
         <f t="shared" si="1"/>
         <v>19/06/23
 au
 25/06/23</v>
       </c>
-      <c r="E44" s="48"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="26"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="10"/>
     </row>
     <row r="45" spans="1:12" ht="32" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="11"/>
@@ -4269,215 +4370,200 @@
         <f t="shared" si="3"/>
         <v>45109</v>
       </c>
-      <c r="D45" s="21" t="str">
+      <c r="D45" s="19" t="str">
         <f t="shared" si="1"/>
         <v>26/06/23
 au
 02/07/23</v>
       </c>
-      <c r="E45" s="23">
+      <c r="E45" s="21">
         <f>E43+1</f>
         <v>18</v>
       </c>
-      <c r="F45" s="51"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
       <c r="L45" s="7"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B46" s="15"/>
+      <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B47" s="15"/>
+      <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B48" s="15"/>
+      <c r="B48" s="14"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B49" s="15"/>
+      <c r="B49" s="14"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B50" s="15"/>
+      <c r="B50" s="14"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B51" s="15"/>
+      <c r="B51" s="14"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B52" s="15"/>
+      <c r="B52" s="14"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B53" s="15"/>
+      <c r="B53" s="14"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B54" s="15"/>
+      <c r="B54" s="14"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B55" s="15"/>
+      <c r="B55" s="14"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B56" s="15"/>
+      <c r="B56" s="14"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B57" s="15"/>
+      <c r="B57" s="14"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B58" s="15"/>
+      <c r="B58" s="14"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B59" s="15"/>
+      <c r="B59" s="14"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B60" s="15"/>
+      <c r="B60" s="14"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B61" s="15"/>
+      <c r="B61" s="14"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B62" s="15"/>
+      <c r="B62" s="14"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B63" s="15"/>
+      <c r="B63" s="14"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B64" s="15"/>
+      <c r="B64" s="14"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B65" s="15"/>
+      <c r="B65" s="14"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B66" s="15"/>
+      <c r="B66" s="14"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B67" s="15"/>
+      <c r="B67" s="14"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B68" s="15"/>
+      <c r="B68" s="14"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B69" s="15"/>
+      <c r="B69" s="14"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B70" s="15"/>
+      <c r="B70" s="14"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B71" s="15"/>
+      <c r="B71" s="14"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B72" s="15"/>
+      <c r="B72" s="14"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B73" s="15"/>
+      <c r="B73" s="14"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B74" s="15"/>
+      <c r="B74" s="14"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B75" s="15"/>
+      <c r="B75" s="14"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B76" s="15"/>
+      <c r="B76" s="14"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B77" s="15"/>
+      <c r="B77" s="14"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B78" s="15"/>
+      <c r="B78" s="14"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B79" s="15"/>
+      <c r="B79" s="14"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B80" s="15"/>
+      <c r="B80" s="14"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B81" s="15"/>
+      <c r="B81" s="14"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B82" s="15"/>
+      <c r="B82" s="14"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B83" s="15"/>
+      <c r="B83" s="14"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B84" s="15"/>
+      <c r="B84" s="14"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B85" s="15"/>
+      <c r="B85" s="14"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B86" s="15"/>
+      <c r="B86" s="14"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B87" s="15"/>
+      <c r="B87" s="14"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B88" s="15"/>
+      <c r="B88" s="14"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B89" s="15"/>
+      <c r="B89" s="14"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B90" s="15"/>
+      <c r="B90" s="14"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B91" s="15"/>
+      <c r="B91" s="14"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B92" s="15"/>
+      <c r="B92" s="14"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B93" s="15"/>
+      <c r="B93" s="14"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B94" s="15"/>
+      <c r="B94" s="14"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B95" s="15"/>
+      <c r="B95" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
-    <mergeCell ref="E2:L2"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="E18:L19"/>
-    <mergeCell ref="E10:L11"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="I23:I24"/>
+  <mergeCells count="71">
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
     <mergeCell ref="E34:L35"/>
     <mergeCell ref="E37:E38"/>
     <mergeCell ref="F37:F38"/>
@@ -4494,21 +4580,37 @@
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="E18:L19"/>
+    <mergeCell ref="E10:L11"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="E2:L2"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="80" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>